<commit_message>
Sorting and Filtering in Tables
</commit_message>
<xml_diff>
--- a/Intermediate I/Week 5/workbook/W5_V3 SortingAndFiltering.xlsx
+++ b/Intermediate I/Week 5/workbook/W5_V3 SortingAndFiltering.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IEUser\Google Drive\Excel MOOC\002 Course 2 - Intermediate I\05 Week 5\01 Workbooks\Actual Recorded\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\foongmin\Desktop\excel-skills-for-business\Intermediate I\Week 5\workbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01BB9AEF-1C33-4153-820D-31A8EACDED16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12080" windowHeight="4290"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Staff" sheetId="1" r:id="rId1"/>
@@ -34,10 +35,18 @@
     <definedName name="Pension_Rate">Staff!$P$1</definedName>
     <definedName name="Years_Service">Staff!$G$4:$G$38</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -562,7 +571,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
@@ -687,7 +696,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -743,6 +752,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent1" xfId="4" builtinId="30"/>
@@ -752,6 +767,17 @@
     <cellStyle name="Title" xfId="1" builtinId="15"/>
   </cellStyles>
   <dxfs count="33">
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -765,123 +791,6 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
@@ -922,18 +831,33 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -988,6 +912,56 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -995,7 +969,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1016,6 +993,44 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3101,37 +3116,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="HR" displayName="HR" ref="A3:O38" dataDxfId="32">
-  <autoFilter ref="A3:O38"/>
-  <sortState ref="A4:O38">
-    <sortCondition descending="1" ref="F3:F38"/>
-  </sortState>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="HR" displayName="HR" ref="A3:O39" totalsRowCount="1" dataDxfId="32">
+  <autoFilter ref="A3:O38" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="15">
-    <tableColumn id="1" name="Emp ID" dataDxfId="31" totalsRowDxfId="2"/>
-    <tableColumn id="2" name="Last"/>
-    <tableColumn id="3" name="First" dataDxfId="30" totalsRowDxfId="3"/>
-    <tableColumn id="4" name="Gender" dataDxfId="29" totalsRowDxfId="4"/>
-    <tableColumn id="5" name="Email">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Emp ID" totalsRowFunction="count" dataDxfId="31" totalsRowDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Last"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="First" dataDxfId="30" totalsRowDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Gender" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Email">
       <calculatedColumnFormula>LOWER(C4&amp;"."&amp;B4&amp;"@pushpin.com")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Date of Hire" dataDxfId="28" totalsRowDxfId="5"/>
-    <tableColumn id="7" name="Years Service" dataDxfId="27" totalsRowDxfId="6">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Date of Hire" dataDxfId="26" totalsRowDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Years Service" totalsRowFunction="average" dataDxfId="24" totalsRowDxfId="1">
       <calculatedColumnFormula>YEARFRAC(F4,TODAY())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Department" dataDxfId="26" totalsRowDxfId="7"/>
-    <tableColumn id="9" name="Location" dataDxfId="25" totalsRowDxfId="8"/>
-    <tableColumn id="10" name="Floor" dataDxfId="24" totalsRowDxfId="9">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Department" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Location" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Floor" dataDxfId="19" totalsRowDxfId="18">
       <calculatedColumnFormula>LEFT(I4,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Extension" dataDxfId="23" totalsRowDxfId="10">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Extension" dataDxfId="17" totalsRowDxfId="16">
       <calculatedColumnFormula>RIGHT(I4,4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Last Review" dataDxfId="22" totalsRowDxfId="11"/>
-    <tableColumn id="13" name="Next Review" dataDxfId="21" totalsRowDxfId="12">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Last Review" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Next Review" dataDxfId="13" totalsRowDxfId="12">
       <calculatedColumnFormula>L4+365</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Annual Salary" dataDxfId="20" totalsRowDxfId="13"/>
-    <tableColumn id="15" name="Pension" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="14">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Annual Salary" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="0"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Pension" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="9">
       <calculatedColumnFormula>N4*Pension_Rate</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3140,22 +3152,22 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A15:D21" totalsRowShown="0">
-  <autoFilter ref="A15:D21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A15:D21" totalsRowShown="0">
+  <autoFilter ref="A15:D21" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="Department" dataDxfId="18"/>
-    <tableColumn id="2" name="Total Salary" dataDxfId="17">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Department" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Total Salary" dataDxfId="7">
       <calculatedColumnFormula>SUMIFS(Annual_Salary,Department,A16)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="M" dataDxfId="16">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="M" dataDxfId="6">
       <calculatedColumnFormula>SUMIFS(Annual_Salary,Department,A16,Gender,$C$15)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="F" dataDxfId="15">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="F" dataDxfId="5">
       <calculatedColumnFormula>SUMIFS(Annual_Salary,Department,A16,Gender,$D$15)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3459,11 +3471,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3545,139 +3557,139 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E4" t="str">
         <f>LOWER(C4&amp;"."&amp;B4&amp;"@pushpin.com")</f>
-        <v>elizabeth.clark@pushpin.com</v>
+        <v>jim.boller@pushpin.com</v>
       </c>
       <c r="F4" s="7">
-        <v>42874</v>
+        <v>41893</v>
       </c>
       <c r="G4" s="4">
         <f ca="1">YEARFRAC(F4,TODAY())</f>
-        <v>0.16111111111111112</v>
+        <v>5.7694444444444448</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="J4" s="6" t="str">
         <f>LEFT(I4,2)</f>
-        <v>02</v>
+        <v>03</v>
       </c>
       <c r="K4" s="6" t="str">
         <f>RIGHT(I4,4)</f>
-        <v>2414</v>
+        <v>2318</v>
       </c>
       <c r="L4" s="7">
-        <v>42720</v>
+        <v>42835</v>
       </c>
       <c r="M4" s="7">
         <f>L4+365</f>
-        <v>43085</v>
+        <v>43200</v>
       </c>
       <c r="N4" s="8">
-        <v>37000</v>
+        <v>62800</v>
       </c>
       <c r="O4" s="16">
         <f>N4*Pension_Rate</f>
-        <v>3330</v>
+        <v>5652</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>145</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>34</v>
+        <v>146</v>
       </c>
       <c r="D5" s="19" t="s">
         <v>166</v>
       </c>
       <c r="E5" t="str">
         <f>LOWER(C5&amp;"."&amp;B5&amp;"@pushpin.com")</f>
-        <v>phoebe.gour@pushpin.com</v>
+        <v>anna.clark@pushpin.com</v>
       </c>
       <c r="F5" s="7">
-        <v>42721</v>
+        <v>41989</v>
       </c>
       <c r="G5" s="4">
         <f ca="1">YEARFRAC(F5,TODAY())</f>
-        <v>0.58333333333333337</v>
+        <v>5.5055555555555555</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="J5" s="6" t="str">
         <f>LEFT(I5,2)</f>
-        <v>02</v>
+        <v>03</v>
       </c>
       <c r="K5" s="6" t="str">
         <f>RIGHT(I5,4)</f>
-        <v>2910</v>
+        <v>2601</v>
       </c>
       <c r="L5" s="7">
-        <v>42539</v>
+        <v>42731</v>
       </c>
       <c r="M5" s="7">
         <f>L5+365</f>
-        <v>42904</v>
+        <v>43096</v>
       </c>
       <c r="N5" s="8">
-        <v>40500</v>
+        <v>58500</v>
       </c>
       <c r="O5" s="16">
         <f>N5*Pension_Rate</f>
-        <v>3645</v>
+        <v>5265</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B6" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E6" t="str">
         <f>LOWER(C6&amp;"."&amp;B6&amp;"@pushpin.com")</f>
-        <v>sean.sanders@pushpin.com</v>
+        <v>alexandra.donnell@pushpin.com</v>
       </c>
       <c r="F6" s="7">
-        <v>42691</v>
+        <v>42228</v>
       </c>
       <c r="G6" s="4">
         <f ca="1">YEARFRAC(F6,TODAY())</f>
-        <v>0.66666666666666663</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J6" s="6" t="str">
         <f>LEFT(I6,2)</f>
@@ -3685,52 +3697,52 @@
       </c>
       <c r="K6" s="6" t="str">
         <f>RIGHT(I6,4)</f>
-        <v>2765</v>
+        <v>2082</v>
       </c>
       <c r="L6" s="7">
-        <v>42566</v>
+        <v>42629</v>
       </c>
       <c r="M6" s="7">
         <f>L6+365</f>
-        <v>42931</v>
+        <v>42994</v>
       </c>
       <c r="N6" s="8">
-        <v>38600</v>
+        <v>54900</v>
       </c>
       <c r="O6" s="16">
         <f>N6*Pension_Rate</f>
-        <v>3474</v>
+        <v>4941</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E7" t="str">
         <f>LOWER(C7&amp;"."&amp;B7&amp;"@pushpin.com")</f>
-        <v>yvette.biti@pushpin.com</v>
+        <v>nicholas.fernandes@pushpin.com</v>
       </c>
       <c r="F7" s="7">
-        <v>42384</v>
+        <v>39023</v>
       </c>
       <c r="G7" s="4">
         <f ca="1">YEARFRAC(F7,TODAY())</f>
-        <v>1.5055555555555555</v>
+        <v>13.627777777777778</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="J7" s="6" t="str">
         <f>LEFT(I7,2)</f>
@@ -3738,105 +3750,105 @@
       </c>
       <c r="K7" s="6" t="str">
         <f>RIGHT(I7,4)</f>
-        <v>2589</v>
+        <v>2372</v>
       </c>
       <c r="L7" s="7">
-        <v>42839</v>
+        <v>42614</v>
       </c>
       <c r="M7" s="7">
         <f>L7+365</f>
-        <v>43204</v>
+        <v>42979</v>
       </c>
       <c r="N7" s="8">
-        <v>51400</v>
+        <v>51600</v>
       </c>
       <c r="O7" s="16">
         <f>N7*Pension_Rate</f>
-        <v>4626</v>
+        <v>4644</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D8" s="19" t="s">
         <v>165</v>
       </c>
       <c r="E8" t="str">
         <f>LOWER(C8&amp;"."&amp;B8&amp;"@pushpin.com")</f>
-        <v>mark.ellis@pushpin.com</v>
+        <v>adam.barry@pushpin.com</v>
       </c>
       <c r="F8" s="7">
-        <v>42371</v>
+        <v>38099</v>
       </c>
       <c r="G8" s="4">
         <f ca="1">YEARFRAC(F8,TODAY())</f>
-        <v>1.5416666666666667</v>
+        <v>16.155555555555555</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="J8" s="6" t="str">
         <f>LEFT(I8,2)</f>
-        <v>03</v>
+        <v>02</v>
       </c>
       <c r="K8" s="6" t="str">
         <f>RIGHT(I8,4)</f>
-        <v>2482</v>
+        <v>2018</v>
       </c>
       <c r="L8" s="7">
-        <v>42619</v>
+        <v>42860</v>
       </c>
       <c r="M8" s="7">
         <f>L8+365</f>
-        <v>42984</v>
+        <v>43225</v>
       </c>
       <c r="N8" s="8">
-        <v>58500</v>
+        <v>59200</v>
       </c>
       <c r="O8" s="16">
         <f>N8*Pension_Rate</f>
-        <v>5265</v>
+        <v>5328</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>145</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="D9" s="19" t="s">
         <v>166</v>
       </c>
       <c r="E9" t="str">
         <f>LOWER(C9&amp;"."&amp;B9&amp;"@pushpin.com")</f>
-        <v>radhya.senome@pushpin.com</v>
+        <v>elizabeth.clark@pushpin.com</v>
       </c>
       <c r="F9" s="7">
-        <v>42324</v>
+        <v>42874</v>
       </c>
       <c r="G9" s="4">
         <f ca="1">YEARFRAC(F9,TODAY())</f>
-        <v>1.6694444444444445</v>
+        <v>3.0805555555555557</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="J9" s="6" t="str">
         <f>LEFT(I9,2)</f>
@@ -3844,52 +3856,52 @@
       </c>
       <c r="K9" s="6" t="str">
         <f>RIGHT(I9,4)</f>
-        <v>2260</v>
+        <v>2414</v>
       </c>
       <c r="L9" s="7">
-        <v>42563</v>
+        <v>42720</v>
       </c>
       <c r="M9" s="7">
         <f>L9+365</f>
-        <v>42928</v>
+        <v>43085</v>
       </c>
       <c r="N9" s="8">
-        <v>35600</v>
+        <v>37000</v>
       </c>
       <c r="O9" s="16">
         <f>N9*Pension_Rate</f>
-        <v>3204</v>
+        <v>3330</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>147</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>115</v>
+        <v>20</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E10" t="str">
         <f>LOWER(C10&amp;"."&amp;B10&amp;"@pushpin.com")</f>
-        <v>peter.staples@pushpin.com</v>
+        <v>sabrina.cole@pushpin.com</v>
       </c>
       <c r="F10" s="7">
-        <v>42321</v>
+        <v>41401</v>
       </c>
       <c r="G10" s="4">
         <f ca="1">YEARFRAC(F10,TODAY())</f>
-        <v>1.6777777777777778</v>
+        <v>7.1138888888888889</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
       <c r="J10" s="6" t="str">
         <f>LEFT(I10,2)</f>
@@ -3897,264 +3909,264 @@
       </c>
       <c r="K10" s="6" t="str">
         <f>RIGHT(I10,4)</f>
-        <v>2654</v>
+        <v>2537</v>
       </c>
       <c r="L10" s="7">
-        <v>42551</v>
+        <v>42710</v>
       </c>
       <c r="M10" s="7">
         <f>L10+365</f>
-        <v>42916</v>
+        <v>43075</v>
       </c>
       <c r="N10" s="8">
-        <v>49600</v>
+        <v>45100</v>
       </c>
       <c r="O10" s="16">
         <f>N10*Pension_Rate</f>
-        <v>4464</v>
+        <v>4059</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>157</v>
+        <v>18</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E11" t="str">
         <f>LOWER(C11&amp;"."&amp;B11&amp;"@pushpin.com")</f>
-        <v>carlos.martinez@pushpin.com</v>
+        <v>janet.comuntzis@pushpin.com</v>
       </c>
       <c r="F11" s="7">
-        <v>42229</v>
+        <v>39686</v>
       </c>
       <c r="G11" s="4">
         <f ca="1">YEARFRAC(F11,TODAY())</f>
-        <v>1.9277777777777778</v>
+        <v>11.811111111111112</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="J11" s="6" t="str">
         <f>LEFT(I11,2)</f>
-        <v>03</v>
+        <v>02</v>
       </c>
       <c r="K11" s="6" t="str">
         <f>RIGHT(I11,4)</f>
-        <v>2764</v>
+        <v>2286</v>
       </c>
       <c r="L11" s="7">
-        <v>42845</v>
+        <v>42658</v>
       </c>
       <c r="M11" s="7">
         <f>L11+365</f>
-        <v>43210</v>
+        <v>43023</v>
       </c>
       <c r="N11" s="8">
-        <v>47900</v>
+        <v>55800</v>
       </c>
       <c r="O11" s="16">
         <f>N11*Pension_Rate</f>
-        <v>4311</v>
+        <v>5022</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="B12" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D12" s="19" t="s">
         <v>166</v>
       </c>
       <c r="E12" t="str">
         <f>LOWER(C12&amp;"."&amp;B12&amp;"@pushpin.com")</f>
-        <v>alexandra.donnell@pushpin.com</v>
+        <v>susan.filosa@pushpin.com</v>
       </c>
       <c r="F12" s="7">
-        <v>42228</v>
+        <v>38744</v>
       </c>
       <c r="G12" s="4">
         <f ca="1">YEARFRAC(F12,TODAY())</f>
-        <v>1.9305555555555556</v>
+        <v>14.391666666666667</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="J12" s="6" t="str">
         <f>LEFT(I12,2)</f>
-        <v>03</v>
+        <v>02</v>
       </c>
       <c r="K12" s="6" t="str">
         <f>RIGHT(I12,4)</f>
-        <v>2082</v>
+        <v>2279</v>
       </c>
       <c r="L12" s="7">
-        <v>42629</v>
+        <v>42596</v>
       </c>
       <c r="M12" s="7">
         <f>L12+365</f>
-        <v>42994</v>
+        <v>42961</v>
       </c>
       <c r="N12" s="8">
-        <v>54900</v>
+        <v>58400</v>
       </c>
       <c r="O12" s="16">
         <f>N12*Pension_Rate</f>
-        <v>4941</v>
+        <v>5256</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>84</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>140</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="D13" s="19" t="s">
         <v>165</v>
       </c>
       <c r="E13" t="str">
         <f>LOWER(C13&amp;"."&amp;B13&amp;"@pushpin.com")</f>
-        <v>leighton.forrest@pushpin.com</v>
+        <v>joe.carol@pushpin.com</v>
       </c>
       <c r="F13" s="7">
-        <v>42120</v>
+        <v>36923</v>
       </c>
       <c r="G13" s="4">
         <f ca="1">YEARFRAC(F13,TODAY())</f>
-        <v>2.2250000000000001</v>
+        <v>19.380555555555556</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="J13" s="6" t="str">
         <f>LEFT(I13,2)</f>
-        <v>02</v>
+        <v>01</v>
       </c>
       <c r="K13" s="6" t="str">
         <f>RIGHT(I13,4)</f>
-        <v>2284</v>
+        <v>2321</v>
       </c>
       <c r="L13" s="7">
-        <v>42586</v>
+        <v>42817</v>
       </c>
       <c r="M13" s="7">
         <f>L13+365</f>
-        <v>42951</v>
+        <v>43182</v>
       </c>
       <c r="N13" s="8">
-        <v>56200</v>
+        <v>101400</v>
       </c>
       <c r="O13" s="16">
         <f>N13*Pension_Rate</f>
-        <v>5058</v>
+        <v>9126</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>159</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="D14" s="19" t="s">
         <v>166</v>
       </c>
       <c r="E14" t="str">
         <f>LOWER(C14&amp;"."&amp;B14&amp;"@pushpin.com")</f>
-        <v>aanya.zhang@pushpin.com</v>
+        <v>mei.wang@pushpin.com</v>
       </c>
       <c r="F14" s="7">
-        <v>42002</v>
+        <v>40188</v>
       </c>
       <c r="G14" s="4">
         <f ca="1">YEARFRAC(F14,TODAY())</f>
-        <v>2.5499999999999998</v>
+        <v>10.438888888888888</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="J14" s="6" t="str">
         <f>LEFT(I14,2)</f>
-        <v>02</v>
+        <v>01</v>
       </c>
       <c r="K14" s="6" t="str">
         <f>RIGHT(I14,4)</f>
-        <v>2793</v>
+        <v>2783</v>
       </c>
       <c r="L14" s="7">
-        <v>42540</v>
+        <v>42544</v>
       </c>
       <c r="M14" s="7">
         <f>L14+365</f>
-        <v>42905</v>
+        <v>42909</v>
       </c>
       <c r="N14" s="8">
-        <v>46500</v>
+        <v>96400</v>
       </c>
       <c r="O14" s="16">
         <f>N14*Pension_Rate</f>
-        <v>4185</v>
+        <v>8676</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B15" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>146</v>
+        <v>27</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E15" t="str">
         <f>LOWER(C15&amp;"."&amp;B15&amp;"@pushpin.com")</f>
-        <v>anna.clark@pushpin.com</v>
+        <v>jim.chaffee@pushpin.com</v>
       </c>
       <c r="F15" s="7">
-        <v>41989</v>
+        <v>41787</v>
       </c>
       <c r="G15" s="4">
         <f ca="1">YEARFRAC(F15,TODAY())</f>
-        <v>2.5861111111111112</v>
+        <v>6.0555555555555554</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="J15" s="6" t="str">
         <f>LEFT(I15,2)</f>
@@ -4162,158 +4174,158 @@
       </c>
       <c r="K15" s="6" t="str">
         <f>RIGHT(I15,4)</f>
-        <v>2601</v>
+        <v>2432</v>
       </c>
       <c r="L15" s="7">
-        <v>42731</v>
+        <v>42804</v>
       </c>
       <c r="M15" s="7">
         <f>L15+365</f>
-        <v>43096</v>
+        <v>43169</v>
       </c>
       <c r="N15" s="8">
-        <v>58500</v>
+        <v>42100</v>
       </c>
       <c r="O15" s="16">
         <f>N15*Pension_Rate</f>
-        <v>5265</v>
+        <v>3789</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>142</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E16" t="str">
         <f>LOWER(C16&amp;"."&amp;B16&amp;"@pushpin.com")</f>
-        <v>connor.betts@pushpin.com</v>
+        <v>uma.chaudri@pushpin.com</v>
       </c>
       <c r="F16" s="7">
-        <v>41956</v>
+        <v>40994</v>
       </c>
       <c r="G16" s="4">
         <f ca="1">YEARFRAC(F16,TODAY())</f>
-        <v>2.6777777777777776</v>
+        <v>8.2277777777777779</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="J16" s="6" t="str">
         <f>LEFT(I16,2)</f>
-        <v>02</v>
+        <v>03</v>
       </c>
       <c r="K16" s="6" t="str">
         <f>RIGHT(I16,4)</f>
-        <v>2347</v>
+        <v>2134</v>
       </c>
       <c r="L16" s="7">
-        <v>42848</v>
+        <v>42776</v>
       </c>
       <c r="M16" s="7">
         <f>L16+365</f>
-        <v>43213</v>
+        <v>43141</v>
       </c>
       <c r="N16" s="8">
-        <v>52600</v>
+        <v>63200</v>
       </c>
       <c r="O16" s="16">
         <f>N16*Pension_Rate</f>
-        <v>4734</v>
+        <v>5688</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>156</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>46</v>
+        <v>157</v>
       </c>
       <c r="D17" s="19" t="s">
         <v>165</v>
       </c>
       <c r="E17" t="str">
         <f>LOWER(C17&amp;"."&amp;B17&amp;"@pushpin.com")</f>
-        <v>charlie.bui@pushpin.com</v>
+        <v>carlos.martinez@pushpin.com</v>
       </c>
       <c r="F17" s="7">
-        <v>41903</v>
+        <v>42229</v>
       </c>
       <c r="G17" s="4">
         <f ca="1">YEARFRAC(F17,TODAY())</f>
-        <v>2.8222222222222224</v>
+        <v>4.8472222222222223</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="J17" s="6" t="str">
         <f>LEFT(I17,2)</f>
-        <v>02</v>
+        <v>03</v>
       </c>
       <c r="K17" s="6" t="str">
         <f>RIGHT(I17,4)</f>
-        <v>2694</v>
+        <v>2764</v>
       </c>
       <c r="L17" s="7">
-        <v>42828</v>
+        <v>42845</v>
       </c>
       <c r="M17" s="7">
         <f>L17+365</f>
-        <v>43193</v>
+        <v>43210</v>
       </c>
       <c r="N17" s="8">
-        <v>54700</v>
+        <v>47900</v>
       </c>
       <c r="O17" s="16">
         <f>N17*Pension_Rate</f>
-        <v>4923</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="B18" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="D18" s="19" t="s">
         <v>165</v>
       </c>
       <c r="E18" t="str">
         <f>LOWER(C18&amp;"."&amp;B18&amp;"@pushpin.com")</f>
-        <v>jim.boller@pushpin.com</v>
+        <v>sean.sanders@pushpin.com</v>
       </c>
       <c r="F18" s="7">
-        <v>41893</v>
+        <v>42691</v>
       </c>
       <c r="G18" s="4">
         <f ca="1">YEARFRAC(F18,TODAY())</f>
-        <v>2.85</v>
+        <v>3.5861111111111112</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="J18" s="6" t="str">
         <f>LEFT(I18,2)</f>
@@ -4321,127 +4333,127 @@
       </c>
       <c r="K18" s="6" t="str">
         <f>RIGHT(I18,4)</f>
-        <v>2318</v>
+        <v>2765</v>
       </c>
       <c r="L18" s="7">
-        <v>42835</v>
+        <v>42566</v>
       </c>
       <c r="M18" s="7">
         <f>L18+365</f>
-        <v>43200</v>
+        <v>42931</v>
       </c>
       <c r="N18" s="8">
-        <v>62800</v>
+        <v>38600</v>
       </c>
       <c r="O18" s="16">
         <f>N18*Pension_Rate</f>
-        <v>5652</v>
+        <v>3474</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B19" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E19" t="str">
         <f>LOWER(C19&amp;"."&amp;B19&amp;"@pushpin.com")</f>
-        <v>jim.chaffee@pushpin.com</v>
+        <v>elizabeth.chu@pushpin.com</v>
       </c>
       <c r="F19" s="7">
-        <v>41787</v>
+        <v>40220</v>
       </c>
       <c r="G19" s="4">
         <f ca="1">YEARFRAC(F19,TODAY())</f>
-        <v>3.1361111111111111</v>
+        <v>10.352777777777778</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J19" s="6" t="str">
         <f>LEFT(I19,2)</f>
-        <v>03</v>
+        <v>01</v>
       </c>
       <c r="K19" s="6" t="str">
         <f>RIGHT(I19,4)</f>
-        <v>2432</v>
+        <v>2425</v>
       </c>
       <c r="L19" s="7">
-        <v>42804</v>
+        <v>42761</v>
       </c>
       <c r="M19" s="7">
         <f>L19+365</f>
-        <v>43169</v>
+        <v>43126</v>
       </c>
       <c r="N19" s="8">
-        <v>42100</v>
+        <v>48400</v>
       </c>
       <c r="O19" s="16">
         <f>N19*Pension_Rate</f>
-        <v>3789</v>
+        <v>4356</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>77</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E20" t="str">
         <f>LOWER(C20&amp;"."&amp;B20&amp;"@pushpin.com")</f>
-        <v>sabrina.cole@pushpin.com</v>
+        <v>eric.chung@pushpin.com</v>
       </c>
       <c r="F20" s="7">
-        <v>41401</v>
+        <v>36949</v>
       </c>
       <c r="G20" s="4">
         <f ca="1">YEARFRAC(F20,TODAY())</f>
-        <v>4.1944444444444446</v>
+        <v>19.308333333333334</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="J20" s="6" t="str">
         <f>LEFT(I20,2)</f>
-        <v>02</v>
+        <v>03</v>
       </c>
       <c r="K20" s="6" t="str">
         <f>RIGHT(I20,4)</f>
-        <v>2537</v>
+        <v>2796</v>
       </c>
       <c r="L20" s="7">
-        <v>42710</v>
+        <v>42731</v>
       </c>
       <c r="M20" s="7">
         <f>L20+365</f>
-        <v>43075</v>
+        <v>43096</v>
       </c>
       <c r="N20" s="8">
-        <v>45100</v>
+        <v>70300</v>
       </c>
       <c r="O20" s="16">
         <f>N20*Pension_Rate</f>
-        <v>4059</v>
+        <v>6327</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.35">
@@ -4466,7 +4478,7 @@
       </c>
       <c r="G21" s="4">
         <f ca="1">YEARFRAC(F21,TODAY())</f>
-        <v>4.7194444444444441</v>
+        <v>7.6388888888888893</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>59</v>
@@ -4519,7 +4531,7 @@
       </c>
       <c r="G22" s="4">
         <f ca="1">YEARFRAC(F22,TODAY())</f>
-        <v>4.8166666666666664</v>
+        <v>7.7361111111111107</v>
       </c>
       <c r="H22" t="s">
         <v>59</v>
@@ -4552,33 +4564,33 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="B23" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E23" t="str">
         <f>LOWER(C23&amp;"."&amp;B23&amp;"@pushpin.com")</f>
-        <v>uma.chaudri@pushpin.com</v>
+        <v>mark.ellis@pushpin.com</v>
       </c>
       <c r="F23" s="7">
-        <v>40994</v>
+        <v>42371</v>
       </c>
       <c r="G23" s="4">
         <f ca="1">YEARFRAC(F23,TODAY())</f>
-        <v>5.3083333333333336</v>
+        <v>4.4611111111111112</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="J23" s="6" t="str">
         <f>LEFT(I23,2)</f>
@@ -4586,52 +4598,52 @@
       </c>
       <c r="K23" s="6" t="str">
         <f>RIGHT(I23,4)</f>
-        <v>2134</v>
+        <v>2482</v>
       </c>
       <c r="L23" s="7">
-        <v>42776</v>
+        <v>42619</v>
       </c>
       <c r="M23" s="7">
         <f>L23+365</f>
-        <v>43141</v>
+        <v>42984</v>
       </c>
       <c r="N23" s="8">
-        <v>63200</v>
+        <v>58500</v>
       </c>
       <c r="O23" s="16">
         <f>N23*Pension_Rate</f>
-        <v>5688</v>
+        <v>5265</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B24" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E24" t="str">
         <f>LOWER(C24&amp;"."&amp;B24&amp;"@pushpin.com")</f>
-        <v>natasha.song@pushpin.com</v>
+        <v>stevie.bacata@pushpin.com</v>
       </c>
       <c r="F24" s="7">
-        <v>40713</v>
+        <v>39551</v>
       </c>
       <c r="G24" s="4">
         <f ca="1">YEARFRAC(F24,TODAY())</f>
-        <v>6.0777777777777775</v>
+        <v>12.180555555555555</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>55</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>129</v>
+        <v>96</v>
       </c>
       <c r="J24" s="6" t="str">
         <f>LEFT(I24,2)</f>
@@ -4639,52 +4651,52 @@
       </c>
       <c r="K24" s="6" t="str">
         <f>RIGHT(I24,4)</f>
-        <v>2578</v>
+        <v>2635</v>
       </c>
       <c r="L24" s="7">
-        <v>42552</v>
+        <v>42507</v>
       </c>
       <c r="M24" s="7">
         <f>L24+365</f>
-        <v>42917</v>
+        <v>42872</v>
       </c>
       <c r="N24" s="8">
-        <v>56000</v>
+        <v>58200</v>
       </c>
       <c r="O24" s="16">
         <f>N24*Pension_Rate</f>
-        <v>5040</v>
+        <v>5238</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E25" t="str">
         <f>LOWER(C25&amp;"."&amp;B25&amp;"@pushpin.com")</f>
-        <v>samantha.chairs@pushpin.com</v>
+        <v>connor.betts@pushpin.com</v>
       </c>
       <c r="F25" s="7">
-        <v>40595</v>
+        <v>41956</v>
       </c>
       <c r="G25" s="4">
         <f ca="1">YEARFRAC(F25,TODAY())</f>
-        <v>6.4055555555555559</v>
+        <v>5.5972222222222223</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>55</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="J25" s="6" t="str">
         <f>LEFT(I25,2)</f>
@@ -4692,158 +4704,158 @@
       </c>
       <c r="K25" s="6" t="str">
         <f>RIGHT(I25,4)</f>
-        <v>2962</v>
+        <v>2347</v>
       </c>
       <c r="L25" s="7">
-        <v>42801</v>
+        <v>42848</v>
       </c>
       <c r="M25" s="7">
         <f>L25+365</f>
-        <v>43166</v>
+        <v>43213</v>
       </c>
       <c r="N25" s="8">
-        <v>59300</v>
+        <v>52600</v>
       </c>
       <c r="O25" s="16">
         <f>N25*Pension_Rate</f>
-        <v>5337</v>
+        <v>4734</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="B26" t="s">
-        <v>143</v>
+        <v>45</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="D26" s="19" t="s">
         <v>166</v>
       </c>
       <c r="E26" t="str">
         <f>LOWER(C26&amp;"."&amp;B26&amp;"@pushpin.com")</f>
-        <v>elizabeth.chu@pushpin.com</v>
+        <v>yvette.biti@pushpin.com</v>
       </c>
       <c r="F26" s="7">
-        <v>40220</v>
+        <v>42384</v>
       </c>
       <c r="G26" s="4">
         <f ca="1">YEARFRAC(F26,TODAY())</f>
-        <v>7.4333333333333336</v>
+        <v>4.4249999999999998</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="J26" s="6" t="str">
         <f>LEFT(I26,2)</f>
-        <v>01</v>
+        <v>02</v>
       </c>
       <c r="K26" s="6" t="str">
         <f>RIGHT(I26,4)</f>
-        <v>2425</v>
+        <v>2589</v>
       </c>
       <c r="L26" s="7">
-        <v>42761</v>
+        <v>42839</v>
       </c>
       <c r="M26" s="7">
         <f>L26+365</f>
-        <v>43126</v>
+        <v>43204</v>
       </c>
       <c r="N26" s="8">
-        <v>48400</v>
+        <v>51400</v>
       </c>
       <c r="O26" s="16">
         <f>N26*Pension_Rate</f>
-        <v>4356</v>
+        <v>4626</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="B27" t="s">
-        <v>159</v>
+        <v>47</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E27" t="str">
         <f>LOWER(C27&amp;"."&amp;B27&amp;"@pushpin.com")</f>
-        <v>mei.wang@pushpin.com</v>
+        <v>charlie.bui@pushpin.com</v>
       </c>
       <c r="F27" s="7">
-        <v>40188</v>
+        <v>41903</v>
       </c>
       <c r="G27" s="4">
         <f ca="1">YEARFRAC(F27,TODAY())</f>
-        <v>7.5194444444444448</v>
+        <v>5.7416666666666663</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="J27" s="6" t="str">
         <f>LEFT(I27,2)</f>
-        <v>01</v>
+        <v>02</v>
       </c>
       <c r="K27" s="6" t="str">
         <f>RIGHT(I27,4)</f>
-        <v>2783</v>
+        <v>2694</v>
       </c>
       <c r="L27" s="7">
-        <v>42544</v>
+        <v>42828</v>
       </c>
       <c r="M27" s="7">
         <f>L27+365</f>
-        <v>42909</v>
+        <v>43193</v>
       </c>
       <c r="N27" s="8">
-        <v>96400</v>
+        <v>54700</v>
       </c>
       <c r="O27" s="16">
         <f>N27*Pension_Rate</f>
-        <v>8676</v>
+        <v>4923</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E28" t="str">
         <f>LOWER(C28&amp;"."&amp;B28&amp;"@pushpin.com")</f>
-        <v>mihael.khan@pushpin.com</v>
+        <v>tina.carlton@pushpin.com</v>
       </c>
       <c r="F28" s="7">
-        <v>40160</v>
+        <v>38798</v>
       </c>
       <c r="G28" s="4">
         <f ca="1">YEARFRAC(F28,TODAY())</f>
-        <v>7.5944444444444441</v>
+        <v>14.238888888888889</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>55</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="J28" s="6" t="str">
         <f>LEFT(I28,2)</f>
@@ -4851,52 +4863,52 @@
       </c>
       <c r="K28" s="6" t="str">
         <f>RIGHT(I28,4)</f>
-        <v>2294</v>
+        <v>2699</v>
       </c>
       <c r="L28" s="7">
-        <v>42566</v>
+        <v>42825</v>
       </c>
       <c r="M28" s="7">
         <f>L28+365</f>
-        <v>42931</v>
+        <v>43190</v>
       </c>
       <c r="N28" s="8">
-        <v>55500</v>
+        <v>59200</v>
       </c>
       <c r="O28" s="16">
         <f>N28*Pension_Rate</f>
-        <v>4995</v>
+        <v>5328</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B29" t="s">
-        <v>148</v>
+        <v>31</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D29" s="19" t="s">
         <v>166</v>
       </c>
       <c r="E29" t="str">
         <f>LOWER(C29&amp;"."&amp;B29&amp;"@pushpin.com")</f>
-        <v>janet.comuntzis@pushpin.com</v>
+        <v>samantha.chairs@pushpin.com</v>
       </c>
       <c r="F29" s="7">
-        <v>39686</v>
+        <v>40595</v>
       </c>
       <c r="G29" s="4">
         <f ca="1">YEARFRAC(F29,TODAY())</f>
-        <v>8.8916666666666675</v>
+        <v>9.3249999999999993</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="J29" s="6" t="str">
         <f>LEFT(I29,2)</f>
@@ -4904,105 +4916,105 @@
       </c>
       <c r="K29" s="6" t="str">
         <f>RIGHT(I29,4)</f>
-        <v>2286</v>
+        <v>2962</v>
       </c>
       <c r="L29" s="7">
-        <v>42658</v>
+        <v>42801</v>
       </c>
       <c r="M29" s="7">
         <f>L29+365</f>
-        <v>43023</v>
+        <v>43166</v>
       </c>
       <c r="N29" s="8">
-        <v>55800</v>
+        <v>59300</v>
       </c>
       <c r="O29" s="16">
         <f>N29*Pension_Rate</f>
-        <v>5022</v>
+        <v>5337</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B30" t="s">
-        <v>49</v>
+        <v>153</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E30" t="str">
         <f>LOWER(C30&amp;"."&amp;B30&amp;"@pushpin.com")</f>
-        <v>stevie.bacata@pushpin.com</v>
+        <v>mary.ferris@pushpin.com</v>
       </c>
       <c r="F30" s="7">
-        <v>39551</v>
+        <v>38548</v>
       </c>
       <c r="G30" s="4">
         <f ca="1">YEARFRAC(F30,TODAY())</f>
-        <v>9.2611111111111111</v>
+        <v>14.925000000000001</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>55</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="J30" s="6" t="str">
         <f>LEFT(I30,2)</f>
-        <v>02</v>
+        <v>03</v>
       </c>
       <c r="K30" s="6" t="str">
         <f>RIGHT(I30,4)</f>
-        <v>2635</v>
+        <v>2392</v>
       </c>
       <c r="L30" s="7">
-        <v>42507</v>
+        <v>42598</v>
       </c>
       <c r="M30" s="7">
         <f>L30+365</f>
-        <v>42872</v>
+        <v>42963</v>
       </c>
       <c r="N30" s="8">
-        <v>58200</v>
+        <v>62900</v>
       </c>
       <c r="O30" s="16">
         <f>N30*Pension_Rate</f>
-        <v>5238</v>
+        <v>5661</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>51</v>
+        <v>155</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>165</v>
       </c>
       <c r="E31" t="str">
         <f>LOWER(C31&amp;"."&amp;B31&amp;"@pushpin.com")</f>
-        <v>nicholas.fernandes@pushpin.com</v>
+        <v>daniel.flanders@pushpin.com</v>
       </c>
       <c r="F31" s="7">
-        <v>39023</v>
+        <v>37510</v>
       </c>
       <c r="G31" s="4">
         <f ca="1">YEARFRAC(F31,TODAY())</f>
-        <v>10.708333333333334</v>
+        <v>17.769444444444446</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="J31" s="6" t="str">
         <f>LEFT(I31,2)</f>
@@ -5010,52 +5022,52 @@
       </c>
       <c r="K31" s="6" t="str">
         <f>RIGHT(I31,4)</f>
-        <v>2372</v>
+        <v>2639</v>
       </c>
       <c r="L31" s="7">
-        <v>42614</v>
+        <v>42590</v>
       </c>
       <c r="M31" s="7">
         <f>L31+365</f>
-        <v>42979</v>
+        <v>42955</v>
       </c>
       <c r="N31" s="8">
-        <v>51600</v>
+        <v>68800</v>
       </c>
       <c r="O31" s="16">
         <f>N31*Pension_Rate</f>
-        <v>4644</v>
+        <v>6192</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="B32" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E32" t="str">
         <f>LOWER(C32&amp;"."&amp;B32&amp;"@pushpin.com")</f>
-        <v>tina.carlton@pushpin.com</v>
+        <v>leighton.forrest@pushpin.com</v>
       </c>
       <c r="F32" s="7">
-        <v>38798</v>
+        <v>42120</v>
       </c>
       <c r="G32" s="4">
         <f ca="1">YEARFRAC(F32,TODAY())</f>
-        <v>11.319444444444445</v>
+        <v>5.1444444444444448</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>55</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="J32" s="6" t="str">
         <f>LEFT(I32,2)</f>
@@ -5063,52 +5075,52 @@
       </c>
       <c r="K32" s="6" t="str">
         <f>RIGHT(I32,4)</f>
-        <v>2699</v>
+        <v>2284</v>
       </c>
       <c r="L32" s="7">
-        <v>42825</v>
+        <v>42586</v>
       </c>
       <c r="M32" s="7">
         <f>L32+365</f>
-        <v>43190</v>
+        <v>42951</v>
       </c>
       <c r="N32" s="8">
-        <v>59200</v>
+        <v>56200</v>
       </c>
       <c r="O32" s="16">
         <f>N32*Pension_Rate</f>
-        <v>5328</v>
+        <v>5058</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="B33" t="s">
-        <v>154</v>
+        <v>35</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="D33" s="19" t="s">
         <v>166</v>
       </c>
       <c r="E33" t="str">
         <f>LOWER(C33&amp;"."&amp;B33&amp;"@pushpin.com")</f>
-        <v>susan.filosa@pushpin.com</v>
+        <v>phoebe.gour@pushpin.com</v>
       </c>
       <c r="F33" s="7">
-        <v>38744</v>
+        <v>42721</v>
       </c>
       <c r="G33" s="4">
         <f ca="1">YEARFRAC(F33,TODAY())</f>
-        <v>11.472222222222221</v>
+        <v>3.5027777777777778</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="J33" s="6" t="str">
         <f>LEFT(I33,2)</f>
@@ -5116,105 +5128,105 @@
       </c>
       <c r="K33" s="6" t="str">
         <f>RIGHT(I33,4)</f>
-        <v>2279</v>
+        <v>2910</v>
       </c>
       <c r="L33" s="7">
-        <v>42596</v>
+        <v>42539</v>
       </c>
       <c r="M33" s="7">
         <f>L33+365</f>
-        <v>42961</v>
+        <v>42904</v>
       </c>
       <c r="N33" s="8">
-        <v>58400</v>
+        <v>40500</v>
       </c>
       <c r="O33" s="16">
         <f>N33*Pension_Rate</f>
-        <v>5256</v>
+        <v>3645</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B34" t="s">
-        <v>153</v>
+        <v>33</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E34" t="str">
         <f>LOWER(C34&amp;"."&amp;B34&amp;"@pushpin.com")</f>
-        <v>mary.ferris@pushpin.com</v>
+        <v>mihael.khan@pushpin.com</v>
       </c>
       <c r="F34" s="7">
-        <v>38548</v>
+        <v>40160</v>
       </c>
       <c r="G34" s="4">
         <f ca="1">YEARFRAC(F34,TODAY())</f>
-        <v>12.005555555555556</v>
+        <v>10.513888888888889</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>55</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="J34" s="6" t="str">
         <f>LEFT(I34,2)</f>
-        <v>03</v>
+        <v>02</v>
       </c>
       <c r="K34" s="6" t="str">
         <f>RIGHT(I34,4)</f>
-        <v>2392</v>
+        <v>2294</v>
       </c>
       <c r="L34" s="7">
-        <v>42598</v>
+        <v>42566</v>
       </c>
       <c r="M34" s="7">
         <f>L34+365</f>
-        <v>42963</v>
+        <v>42931</v>
       </c>
       <c r="N34" s="8">
-        <v>62900</v>
+        <v>55500</v>
       </c>
       <c r="O34" s="16">
         <f>N34*Pension_Rate</f>
-        <v>5661</v>
+        <v>4995</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="B35" t="s">
-        <v>138</v>
+        <v>54</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E35" t="str">
         <f>LOWER(C35&amp;"."&amp;B35&amp;"@pushpin.com")</f>
-        <v>adam.barry@pushpin.com</v>
+        <v>radhya.senome@pushpin.com</v>
       </c>
       <c r="F35" s="7">
-        <v>38099</v>
+        <v>42324</v>
       </c>
       <c r="G35" s="4">
         <f ca="1">YEARFRAC(F35,TODAY())</f>
-        <v>13.236111111111111</v>
+        <v>4.5888888888888886</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>97</v>
+        <v>128</v>
       </c>
       <c r="J35" s="6" t="str">
         <f>LEFT(I35,2)</f>
@@ -5222,52 +5234,52 @@
       </c>
       <c r="K35" s="6" t="str">
         <f>RIGHT(I35,4)</f>
-        <v>2018</v>
+        <v>2260</v>
       </c>
       <c r="L35" s="7">
-        <v>42860</v>
+        <v>42563</v>
       </c>
       <c r="M35" s="7">
         <f>L35+365</f>
-        <v>43225</v>
+        <v>42928</v>
       </c>
       <c r="N35" s="8">
-        <v>59200</v>
+        <v>35600</v>
       </c>
       <c r="O35" s="16">
         <f>N35*Pension_Rate</f>
-        <v>5328</v>
+        <v>3204</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="B36" t="s">
-        <v>155</v>
+        <v>39</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E36" t="str">
         <f>LOWER(C36&amp;"."&amp;B36&amp;"@pushpin.com")</f>
-        <v>daniel.flanders@pushpin.com</v>
+        <v>natasha.song@pushpin.com</v>
       </c>
       <c r="F36" s="7">
-        <v>37510</v>
+        <v>40713</v>
       </c>
       <c r="G36" s="4">
         <f ca="1">YEARFRAC(F36,TODAY())</f>
-        <v>14.85</v>
+        <v>8.9972222222222218</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>55</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="J36" s="6" t="str">
         <f>LEFT(I36,2)</f>
@@ -5275,131 +5287,154 @@
       </c>
       <c r="K36" s="6" t="str">
         <f>RIGHT(I36,4)</f>
-        <v>2639</v>
+        <v>2578</v>
       </c>
       <c r="L36" s="7">
-        <v>42590</v>
+        <v>42552</v>
       </c>
       <c r="M36" s="7">
         <f>L36+365</f>
-        <v>42955</v>
+        <v>42917</v>
       </c>
       <c r="N36" s="8">
-        <v>68800</v>
+        <v>56000</v>
       </c>
       <c r="O36" s="16">
         <f>N36*Pension_Rate</f>
-        <v>6192</v>
+        <v>5040</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
-        <v>9</v>
+        <v>87</v>
       </c>
       <c r="B37" t="s">
-        <v>144</v>
+        <v>53</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>56</v>
+        <v>115</v>
       </c>
       <c r="D37" s="19" t="s">
         <v>165</v>
       </c>
       <c r="E37" t="str">
         <f>LOWER(C37&amp;"."&amp;B37&amp;"@pushpin.com")</f>
-        <v>eric.chung@pushpin.com</v>
+        <v>peter.staples@pushpin.com</v>
       </c>
       <c r="F37" s="7">
-        <v>36949</v>
+        <v>42321</v>
       </c>
       <c r="G37" s="4">
         <f ca="1">YEARFRAC(F37,TODAY())</f>
-        <v>16.388888888888889</v>
+        <v>4.5972222222222223</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>105</v>
+        <v>130</v>
       </c>
       <c r="J37" s="6" t="str">
         <f>LEFT(I37,2)</f>
-        <v>03</v>
+        <v>02</v>
       </c>
       <c r="K37" s="6" t="str">
         <f>RIGHT(I37,4)</f>
-        <v>2796</v>
+        <v>2654</v>
       </c>
       <c r="L37" s="7">
-        <v>42731</v>
+        <v>42551</v>
       </c>
       <c r="M37" s="7">
         <f>L37+365</f>
-        <v>43096</v>
+        <v>42916</v>
       </c>
       <c r="N37" s="8">
-        <v>70300</v>
+        <v>49600</v>
       </c>
       <c r="O37" s="16">
         <f>N37*Pension_Rate</f>
-        <v>6327</v>
+        <v>4464</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="B38" t="s">
-        <v>140</v>
+        <v>41</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E38" t="str">
         <f>LOWER(C38&amp;"."&amp;B38&amp;"@pushpin.com")</f>
-        <v>joe.carol@pushpin.com</v>
+        <v>aanya.zhang@pushpin.com</v>
       </c>
       <c r="F38" s="7">
-        <v>36923</v>
+        <v>42002</v>
       </c>
       <c r="G38" s="4">
         <f ca="1">YEARFRAC(F38,TODAY())</f>
-        <v>16.461111111111112</v>
+        <v>5.4694444444444441</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="J38" s="6" t="str">
         <f>LEFT(I38,2)</f>
-        <v>01</v>
+        <v>02</v>
       </c>
       <c r="K38" s="6" t="str">
         <f>RIGHT(I38,4)</f>
-        <v>2321</v>
+        <v>2793</v>
       </c>
       <c r="L38" s="7">
-        <v>42817</v>
+        <v>42540</v>
       </c>
       <c r="M38" s="7">
         <f>L38+365</f>
-        <v>43182</v>
+        <v>42905</v>
       </c>
       <c r="N38" s="8">
-        <v>101400</v>
+        <v>46500</v>
       </c>
       <c r="O38" s="16">
         <f>N38*Pension_Rate</f>
-        <v>9126</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="E40" s="13"/>
+        <v>4185</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A39" s="3">
+        <f>SUBTOTAL(103,HR[Emp ID])</f>
+        <v>35</v>
+      </c>
+      <c r="C39" s="2"/>
+      <c r="D39" s="19"/>
+      <c r="G39" s="4">
+        <f ca="1">SUBTOTAL(101,HR[Years Service])</f>
+        <v>8.8958730158730166</v>
+      </c>
+      <c r="H39" s="21"/>
+      <c r="I39" s="22"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="8">
+        <f>SUBTOTAL(109,HR[Annual Salary])</f>
+        <v>1958400</v>
+      </c>
+      <c r="O39" s="16">
+        <f>SUBTOTAL(109,HR[Pension])</f>
+        <v>176256</v>
+      </c>
     </row>
     <row r="41" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E41" s="13"/>
@@ -5407,15 +5442,18 @@
     <row r="42" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E42" s="13"/>
     </row>
+    <row r="43" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="E43" s="13"/>
+    </row>
   </sheetData>
-  <sortState ref="A4:N38">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:N38">
     <sortCondition ref="A7"/>
   </sortState>
   <conditionalFormatting sqref="M4:M38">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>M4&lt;TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5428,7 +5466,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -5482,7 +5520,7 @@
       </c>
       <c r="B6" s="11">
         <f ca="1">MAX(Years_Service)</f>
-        <v>16.461111111111112</v>
+        <v>19.380555555555556</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>